<commit_message>
Updated num citations of `Generative Adversarial Nets'
</commit_message>
<xml_diff>
--- a/background study/num_citations_of_gan_paper_by_year.xlsx
+++ b/background study/num_citations_of_gan_paper_by_year.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Uni/Graduate/CS 848/final project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Uni/Graduate/CS 848/final project/background study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA9627D8-4A5D-2342-952C-24D1D7936A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25170475-4A46-FB4E-83A8-9079C41B3C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{2B38AC0E-BAC1-F14E-A506-112546E4AFA2}"/>
+    <workbookView xWindow="560" yWindow="2220" windowWidth="28800" windowHeight="16520" xr2:uid="{2B38AC0E-BAC1-F14E-A506-112546E4AFA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$13</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$A$2:$A$13</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">Sheet1!$B$2:$B$13</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$13</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$13</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$13</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$13</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$2:$A$13</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$2:$B$13</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -113,10 +114,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="108"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="8"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -127,7 +128,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -140,14 +141,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400" b="1"/>
               <a:t>Number of Citations of "Generative Adversarial Nets"</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
               <a:t> By Goodfellow et al. Over Time</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2400" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -164,7 +165,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -203,7 +204,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -214,11 +215,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -239,7 +240,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -395,23 +396,10 @@
         <c:axId val="1720238319"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2022"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -419,7 +407,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -432,7 +420,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
                   <a:t>Year</a:t>
                 </a:r>
               </a:p>
@@ -451,7 +439,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -489,7 +477,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -536,7 +524,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -549,7 +537,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600" b="1"/>
                   <a:t>Number of Citations</a:t>
                 </a:r>
               </a:p>
@@ -568,7 +556,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -606,7 +594,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -671,42 +659,8 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
   <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -1236,10 +1190,10 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1268,7 +1222,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1556,7 +1510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1567,7 +1521,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1607,7 +1561,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f t="shared" ref="A5:A14" si="0">A4+1</f>
+        <f t="shared" ref="A5:A13" si="0">A4+1</f>
         <v>2015</v>
       </c>
       <c r="B5">

</xml_diff>